<commit_message>
PROS-4783 - CCRU - CCH Integration - Templates alignment
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
@@ -13,20 +13,19 @@
     <sheet name="Alcomarket" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$40</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1356,21 +1355,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR65536"/>
+  <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O46" activeCellId="0" sqref="O46"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="14" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4760,8 +4758,8 @@
       <c r="AQ39" s="47"/>
       <c r="AR39" s="22"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="53" t="n">
+    <row r="40" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="45" t="s">
@@ -5221,19 +5219,8 @@
       <c r="AP45" s="81"/>
       <c r="AQ45" s="81"/>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:AQ40"/>
+  <autoFilter ref="A1:AQ41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5253,7 +5240,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A40 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5290,7 +5277,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A40 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
CCRU to CCRU_SAND copy
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
@@ -1095,9 +1095,9 @@
   <dimension ref="A1:AR45"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N26" activeCellId="0" sqref="N26:O27"/>
+      <selection pane="bottomLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.45"/>
@@ -4977,7 +4977,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N26:O27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5014,7 +5014,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N26:O27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
PROS-6581 - CCRU - Copy PROD to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Canteen PoS 2018.xlsx
@@ -29,6 +29,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Canteen!$A$1:$AQ$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -255,16 +257,16 @@
     <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprite - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 0.33л</t>
+    <t xml:space="preserve">Sprite - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.25л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин – 0.25л</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 2</t>
@@ -388,7 +390,7 @@
     <t xml:space="preserve">Добрый - Апельсин - 0.33л</t>
   </si>
   <si>
-    <t xml:space="preserve">Moya Semya - Apple mix - 0.175L</t>
+    <t xml:space="preserve">Moya Semya - Apple Mix - 0.175L</t>
   </si>
   <si>
     <t xml:space="preserve">Моя Семья - Яблочный Микс - 0.175л</t>
@@ -938,9 +940,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -950,9 +952,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1094,17 +1096,17 @@
   </sheetPr>
   <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.5465587044534"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="43.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="15.5465587044534"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="47.417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="16.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="62.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1770,7 +1772,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="20" t="s">
         <v>69</v>
       </c>
       <c r="H8" s="13" t="s">
@@ -1785,11 +1787,11 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="9" t="n">
-        <v>5449000014535</v>
+      <c r="O8" s="22" t="n">
+        <v>5449000000729</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
@@ -1858,7 +1860,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="20" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="13" t="s">
@@ -1873,11 +1875,11 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
+      <c r="N9" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="9" t="n">
-        <v>5449000011527</v>
+      <c r="O9" s="22" t="n">
+        <v>5449000000712</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
@@ -3306,10 +3308,10 @@
         <v>73</v>
       </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="23" t="s">
         <v>110</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -3394,10 +3396,10 @@
         <v>73</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="23" t="s">
         <v>114</v>
       </c>
       <c r="I27" s="8" t="s">
@@ -4976,13 +4978,13 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5013,13 +5015,13 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>